<commit_message>
tag v 1.0.0 issue 2 issue 3
</commit_message>
<xml_diff>
--- a/ExcelFile.net.Example.net40/B.xlsx
+++ b/ExcelFile.net.Example.net40/B.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1790" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="2350" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,15 +16,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>{s-Name}</t>
+    <t>Merry Christmas!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{s-Age}</t>
+    <t>{s.Name}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Merry Christmas!</t>
+    <t>{s.Age}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -387,13 +387,13 @@
   <sheetData>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>